<commit_message>
added 3D models to KiCad
Added 3D Models of components to both KiCad Boards

Fixed footprint of screw terminal to match with 30.702 on both easyeda and kicad files

re-rendered 2D view from EasyEDA and  added 3D view rendering from KiCad

Renders in separate folder

Exported new gerbers from both EasyEDA and KiCad with updated footprint

Exported 3D model of both boards from KiCad and added to folder.

Updated link to smd LED to active part.
</commit_message>
<xml_diff>
--- a/6502 ROR Test Board BOM V2.0S.xlsx
+++ b/6502 ROR Test Board BOM V2.0S.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tony\Downloads\6502 ROR Test Board\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tony\Documents\GitHub\6502-ROR-Test-Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06902363-5A7A-46A2-9198-E964500D1A16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{102A87CB-0291-47DC-9F58-F10A7B97A090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BF81D018-8F28-45BB-9BEF-AA2F6781CE47}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="19543" windowHeight="12497" xr2:uid="{BF81D018-8F28-45BB-9BEF-AA2F6781CE47}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -125,15 +125,9 @@
     <t xml:space="preserve">0603 LED </t>
   </si>
   <si>
-    <t>https://www.lcsc.com/product-detail/Light-Emitting-Diodes-LED_Everlight-Elec-19-217-R6C-AL1M2VY-3T_C72044.html</t>
-  </si>
-  <si>
     <t>2N7002</t>
   </si>
   <si>
-    <t>https://www.mouser.com/ProductDetail/Nexperia/2N7002NXBKR?qs=%252B6g0mu59x7J2ddJstTJGkQ%3D%3D</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/en/products/detail/meritek/MA1206XR104K101/20116994</t>
   </si>
   <si>
@@ -147,6 +141,12 @@
   </si>
   <si>
     <t>SN74HCS74DR</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/harvatek-corporation/B19Y1USD-20C000113U1930/16602930</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mouser.com/ProductDetail/Nexperia/2N7002NXBKR?qs=%252B6g0mu59x7J2ddJstTJGkQ%3D%3D </t>
   </si>
 </sst>
 </file>
@@ -573,17 +573,17 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
-    <col min="3" max="3" width="164.85546875" customWidth="1"/>
+    <col min="1" max="1" width="21.53515625" customWidth="1"/>
+    <col min="2" max="2" width="14.15234375" customWidth="1"/>
+    <col min="3" max="3" width="164.84375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -594,7 +594,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -605,7 +605,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -621,7 +621,7 @@
       <c r="F3" s="14"/>
       <c r="G3" s="14"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -629,55 +629,55 @@
         <v>6</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E4" s="14"/>
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="2">
         <v>2</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="E5" s="14"/>
       <c r="F5" s="14"/>
       <c r="G5" s="14"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B6" s="8">
         <v>1</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E6" s="14"/>
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B7" s="2">
         <v>1</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E7" s="14"/>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -691,7 +691,7 @@
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -702,7 +702,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" s="2">
         <v>6502</v>
       </c>
@@ -711,7 +711,7 @@
       </c>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
         <v>28</v>
       </c>
@@ -719,10 +719,10 @@
         <v>2</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>13</v>
       </c>
@@ -733,19 +733,19 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" s="9"/>
       <c r="B13" s="9"/>
       <c r="C13" s="10"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" s="13" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
         <v>26</v>
       </c>
@@ -756,7 +756,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
         <v>6</v>
       </c>
@@ -767,24 +767,24 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
       <c r="C18" s="11"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A19" s="9"/>
       <c r="B19" s="9"/>
       <c r="C19" s="11"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A20" s="12" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="12"/>
       <c r="C20" s="12"/>
     </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
         <v>8</v>
       </c>
@@ -795,7 +795,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
         <v>10</v>
       </c>
@@ -806,14 +806,14 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A25" s="12" t="s">
         <v>21</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="12"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A26" s="7" t="s">
         <v>15</v>
       </c>
@@ -824,7 +824,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A27" s="7" t="s">
         <v>17</v>
       </c>
@@ -852,8 +852,10 @@
     <hyperlink ref="C2" r:id="rId7" xr:uid="{8EF5C484-2D5A-46E3-BCFB-10158E34359E}"/>
     <hyperlink ref="C7" r:id="rId8" xr:uid="{509E168D-67FD-4FCB-B509-BFAC458BF25B}"/>
     <hyperlink ref="C6" r:id="rId9" xr:uid="{63C365A3-7262-4AD6-AC3C-56BD45A3F931}"/>
+    <hyperlink ref="C11" r:id="rId10" xr:uid="{27A66306-D510-415C-A70A-54DD2FEDEC24}"/>
+    <hyperlink ref="C5" r:id="rId11" xr:uid="{AD1D1E6B-D81F-4672-8BDD-965D3856E9D5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId10"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>